<commit_message>
some data to test cases and few documentation
</commit_message>
<xml_diff>
--- a/current status.xlsx
+++ b/current status.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="60" windowWidth="20730" windowHeight="11700"/>
   </bookViews>
@@ -63,9 +63,6 @@
     <t>Программная документация</t>
   </si>
   <si>
-    <t>авто + скрины + отчет с дженкинса + кейсы на анализ азполнить расчетными данными</t>
-  </si>
-  <si>
     <t>Обоснование темы</t>
   </si>
   <si>
@@ -88,12 +85,16 @@
   </si>
   <si>
     <t>На сдачу</t>
+  </si>
+  <si>
+    <t>авто + скрины + отчет с дженкинса + 
+добавить столбцы с оценками</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -232,10 +233,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Нейтральный" xfId="3" builtinId="28"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Плохой" xfId="2" builtinId="27"/>
-    <cellStyle name="Хороший" xfId="1" builtinId="26"/>
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -505,7 +506,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -516,7 +517,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,7 +538,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -570,17 +571,17 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="10"/>
+        <v>20</v>
+      </c>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="2"/>
@@ -588,7 +589,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="2"/>
@@ -596,7 +597,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="2"/>
@@ -604,7 +605,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="2"/>
@@ -612,7 +613,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="2"/>
@@ -624,17 +625,17 @@
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="2" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D12" s="10"/>
     </row>

</xml_diff>